<commit_message>
Update CDEs + 2 neue qualitative/kategoriale CDE (ethnicity & gender assigned at birth)
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cls-l0-activity.xlsx
+++ b/output/StructureDefinition-cls-l0-activity.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2464" uniqueCount="538">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-04T20:22:12+01:00</t>
+    <t>2023-03-05T01:48:17+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -654,11 +654,14 @@
     <t>http://hl7.org/fhir/ValueSet/observation-category</t>
   </si>
   <si>
-    <t>value:$this.code}
-value:$this.system}</t>
+    <t xml:space="preserve">value:coding.code}
+</t>
   </si>
   <si>
     <t>Slice based on the coding.code &amp; coding.system to allow multiple classifications of data elements.</t>
+  </si>
+  <si>
+    <t>openAtEnd</t>
   </si>
   <si>
     <t>CE/CNE/CWE</t>
@@ -3838,10 +3841,10 @@
         <v>205</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>196</v>
@@ -3865,13 +3868,13 @@
         <v>82</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AO15" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AP15" t="s" s="2">
         <v>82</v>
@@ -3879,13 +3882,13 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s" s="2">
         <v>196</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D16" t="s" s="2">
         <v>82</v>
@@ -3919,7 +3922,7 @@
         <v>200</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>82</v>
@@ -3989,13 +3992,13 @@
         <v>82</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AP16" t="s" s="2">
         <v>82</v>
@@ -4003,10 +4006,10 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -4029,13 +4032,13 @@
         <v>82</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -4086,7 +4089,7 @@
         <v>82</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>80</v>
@@ -4121,10 +4124,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -4153,7 +4156,7 @@
         <v>141</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="N18" t="s" s="2">
         <v>143</v>
@@ -4206,7 +4209,7 @@
         <v>146</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>80</v>
@@ -4241,10 +4244,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -4252,13 +4255,13 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>81</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>82</v>
@@ -4267,19 +4270,19 @@
         <v>93</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>82</v>
@@ -4328,7 +4331,7 @@
         <v>82</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>80</v>
@@ -4349,10 +4352,10 @@
         <v>82</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>82</v>
@@ -4363,10 +4366,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -4389,13 +4392,13 @@
         <v>82</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -4446,7 +4449,7 @@
         <v>82</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>80</v>
@@ -4481,10 +4484,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4513,7 +4516,7 @@
         <v>141</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="N21" t="s" s="2">
         <v>143</v>
@@ -4566,7 +4569,7 @@
         <v>146</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>80</v>
@@ -4601,10 +4604,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4612,13 +4615,13 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I22" t="s" s="2">
         <v>82</v>
@@ -4630,23 +4633,23 @@
         <v>108</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="S22" t="s" s="2">
         <v>82</v>
@@ -4688,7 +4691,7 @@
         <v>82</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>80</v>
@@ -4709,10 +4712,10 @@
         <v>82</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>82</v>
@@ -4723,10 +4726,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4749,16 +4752,16 @@
         <v>93</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -4808,7 +4811,7 @@
         <v>82</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>80</v>
@@ -4829,10 +4832,10 @@
         <v>82</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>82</v>
@@ -4843,10 +4846,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4854,13 +4857,13 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I24" t="s" s="2">
         <v>82</v>
@@ -4872,23 +4875,23 @@
         <v>115</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="S24" t="s" s="2">
         <v>82</v>
@@ -4930,7 +4933,7 @@
         <v>82</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>80</v>
@@ -4951,10 +4954,10 @@
         <v>82</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>82</v>
@@ -4965,10 +4968,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4991,19 +4994,19 @@
         <v>93</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>82</v>
@@ -5052,7 +5055,7 @@
         <v>82</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>80</v>
@@ -5073,10 +5076,10 @@
         <v>82</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>82</v>
@@ -5087,10 +5090,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -5113,19 +5116,19 @@
         <v>93</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>82</v>
@@ -5174,7 +5177,7 @@
         <v>82</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>80</v>
@@ -5195,10 +5198,10 @@
         <v>82</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>82</v>
@@ -5209,10 +5212,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -5235,19 +5238,19 @@
         <v>93</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>82</v>
@@ -5296,7 +5299,7 @@
         <v>82</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>80</v>
@@ -5317,10 +5320,10 @@
         <v>82</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>82</v>
@@ -5331,14 +5334,14 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
@@ -5360,16 +5363,16 @@
         <v>197</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>82</v>
@@ -5394,13 +5397,13 @@
         <v>82</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>82</v>
@@ -5418,7 +5421,7 @@
         <v>82</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>92</v>
@@ -5433,30 +5436,30 @@
         <v>105</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AP28" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5479,19 +5482,19 @@
         <v>93</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>82</v>
@@ -5540,7 +5543,7 @@
         <v>82</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>80</v>
@@ -5555,19 +5558,19 @@
         <v>170</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AP29" t="s" s="2">
         <v>82</v>
@@ -5575,10 +5578,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5601,16 +5604,16 @@
         <v>93</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5660,7 +5663,7 @@
         <v>82</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>80</v>
@@ -5681,13 +5684,13 @@
         <v>82</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AP30" t="s" s="2">
         <v>82</v>
@@ -5695,14 +5698,14 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -5721,19 +5724,19 @@
         <v>93</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>82</v>
@@ -5782,7 +5785,7 @@
         <v>82</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>80</v>
@@ -5797,19 +5800,19 @@
         <v>170</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AP31" t="s" s="2">
         <v>82</v>
@@ -5817,14 +5820,14 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -5843,19 +5846,19 @@
         <v>93</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="O32" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>82</v>
@@ -5904,7 +5907,7 @@
         <v>82</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>80</v>
@@ -5919,19 +5922,19 @@
         <v>105</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AP32" t="s" s="2">
         <v>82</v>
@@ -5939,10 +5942,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5965,16 +5968,16 @@
         <v>93</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -6024,7 +6027,7 @@
         <v>82</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>80</v>
@@ -6045,13 +6048,13 @@
         <v>82</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AP33" t="s" s="2">
         <v>82</v>
@@ -6059,10 +6062,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -6085,19 +6088,19 @@
         <v>93</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N34" t="s" s="2">
         <v>168</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>82</v>
@@ -6146,7 +6149,7 @@
         <v>82</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>80</v>
@@ -6161,19 +6164,19 @@
         <v>170</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AP34" t="s" s="2">
         <v>82</v>
@@ -6181,10 +6184,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -6207,19 +6210,19 @@
         <v>93</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="O35" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="P35" t="s" s="2">
         <v>82</v>
@@ -6268,7 +6271,7 @@
         <v>82</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>80</v>
@@ -6277,7 +6280,7 @@
         <v>92</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>105</v>
@@ -6286,27 +6289,27 @@
         <v>82</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP35" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6332,16 +6335,16 @@
         <v>197</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>82</v>
@@ -6366,13 +6369,13 @@
         <v>82</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Z36" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>82</v>
@@ -6390,7 +6393,7 @@
         <v>82</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>80</v>
@@ -6399,7 +6402,7 @@
         <v>92</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>105</v>
@@ -6414,7 +6417,7 @@
         <v>106</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>82</v>
@@ -6425,14 +6428,14 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s" s="2">
@@ -6454,16 +6457,16 @@
         <v>197</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>82</v>
@@ -6488,13 +6491,13 @@
         <v>82</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>82</v>
@@ -6512,7 +6515,7 @@
         <v>82</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>80</v>
@@ -6530,27 +6533,27 @@
         <v>82</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP37" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6573,19 +6576,19 @@
         <v>82</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>82</v>
@@ -6634,7 +6637,7 @@
         <v>82</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>80</v>
@@ -6655,10 +6658,10 @@
         <v>82</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>82</v>
@@ -6669,10 +6672,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6698,13 +6701,13 @@
         <v>197</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6730,13 +6733,13 @@
         <v>82</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="Z39" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>82</v>
@@ -6754,7 +6757,7 @@
         <v>82</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>80</v>
@@ -6772,27 +6775,27 @@
         <v>82</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP39" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6818,16 +6821,16 @@
         <v>197</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="O40" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>82</v>
@@ -6852,13 +6855,13 @@
         <v>82</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>82</v>
@@ -6876,7 +6879,7 @@
         <v>82</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>80</v>
@@ -6897,10 +6900,10 @@
         <v>82</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>82</v>
@@ -6911,10 +6914,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6937,16 +6940,16 @@
         <v>82</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6996,7 +6999,7 @@
         <v>82</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>80</v>
@@ -7014,27 +7017,27 @@
         <v>82</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP41" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -7057,16 +7060,16 @@
         <v>82</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -7116,7 +7119,7 @@
         <v>82</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>80</v>
@@ -7134,27 +7137,27 @@
         <v>82</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP42" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -7177,19 +7180,19 @@
         <v>82</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>82</v>
@@ -7238,7 +7241,7 @@
         <v>82</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>80</v>
@@ -7250,7 +7253,7 @@
         <v>104</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>82</v>
@@ -7259,10 +7262,10 @@
         <v>82</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>82</v>
@@ -7273,10 +7276,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7299,13 +7302,13 @@
         <v>82</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -7356,7 +7359,7 @@
         <v>82</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>80</v>
@@ -7391,10 +7394,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7423,7 +7426,7 @@
         <v>141</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="N45" t="s" s="2">
         <v>143</v>
@@ -7476,7 +7479,7 @@
         <v>146</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>80</v>
@@ -7511,14 +7514,14 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -7540,10 +7543,10 @@
         <v>140</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="N46" t="s" s="2">
         <v>143</v>
@@ -7598,7 +7601,7 @@
         <v>82</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>80</v>
@@ -7633,10 +7636,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7659,16 +7662,16 @@
         <v>82</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -7718,7 +7721,7 @@
         <v>82</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>80</v>
@@ -7727,10 +7730,10 @@
         <v>92</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>82</v>
@@ -7739,10 +7742,10 @@
         <v>82</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>82</v>
@@ -7753,10 +7756,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7779,16 +7782,16 @@
         <v>82</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -7838,7 +7841,7 @@
         <v>82</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>80</v>
@@ -7847,10 +7850,10 @@
         <v>92</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>82</v>
@@ -7859,10 +7862,10 @@
         <v>82</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>82</v>
@@ -7873,10 +7876,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7902,16 +7905,16 @@
         <v>197</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="O49" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>82</v>
@@ -7939,10 +7942,10 @@
         <v>119</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>82</v>
@@ -7960,7 +7963,7 @@
         <v>82</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>80</v>
@@ -7978,13 +7981,13 @@
         <v>82</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>82</v>
@@ -7995,10 +7998,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -8024,16 +8027,16 @@
         <v>197</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="O50" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>82</v>
@@ -8058,13 +8061,13 @@
         <v>82</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>82</v>
@@ -8082,7 +8085,7 @@
         <v>82</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>80</v>
@@ -8100,13 +8103,13 @@
         <v>82</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>82</v>
@@ -8117,10 +8120,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -8143,19 +8146,19 @@
         <v>82</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="O51" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>82</v>
@@ -8204,7 +8207,7 @@
         <v>82</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>80</v>
@@ -8216,7 +8219,7 @@
         <v>104</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>82</v>
@@ -8225,10 +8228,10 @@
         <v>82</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="AO51" t="s" s="2">
         <v>82</v>
@@ -8239,10 +8242,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8265,16 +8268,16 @@
         <v>82</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -8324,7 +8327,7 @@
         <v>82</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>80</v>
@@ -8345,10 +8348,10 @@
         <v>82</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>82</v>
@@ -8359,10 +8362,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8385,16 +8388,16 @@
         <v>93</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -8444,7 +8447,7 @@
         <v>82</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>80</v>
@@ -8465,10 +8468,10 @@
         <v>82</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>82</v>
@@ -8479,10 +8482,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8505,16 +8508,16 @@
         <v>93</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -8564,7 +8567,7 @@
         <v>82</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>80</v>
@@ -8585,10 +8588,10 @@
         <v>82</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="AO54" t="s" s="2">
         <v>82</v>
@@ -8599,10 +8602,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8625,19 +8628,19 @@
         <v>93</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="O55" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="P55" t="s" s="2">
         <v>82</v>
@@ -8686,7 +8689,7 @@
         <v>82</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>80</v>
@@ -8707,10 +8710,10 @@
         <v>82</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="AO55" t="s" s="2">
         <v>82</v>
@@ -8721,10 +8724,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8747,13 +8750,13 @@
         <v>82</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8804,7 +8807,7 @@
         <v>82</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>80</v>
@@ -8839,10 +8842,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8871,7 +8874,7 @@
         <v>141</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="N57" t="s" s="2">
         <v>143</v>
@@ -8924,7 +8927,7 @@
         <v>146</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>80</v>
@@ -8959,14 +8962,14 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
@@ -8988,10 +8991,10 @@
         <v>140</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="N58" t="s" s="2">
         <v>143</v>
@@ -9046,7 +9049,7 @@
         <v>82</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>80</v>
@@ -9081,10 +9084,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9110,16 +9113,16 @@
         <v>197</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="O59" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="P59" t="s" s="2">
         <v>82</v>
@@ -9144,13 +9147,13 @@
         <v>82</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>82</v>
@@ -9168,7 +9171,7 @@
         <v>82</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>92</v>
@@ -9186,16 +9189,16 @@
         <v>82</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AP59" t="s" s="2">
         <v>82</v>
@@ -9203,10 +9206,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9229,19 +9232,19 @@
         <v>93</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="O60" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="P60" t="s" s="2">
         <v>82</v>
@@ -9290,7 +9293,7 @@
         <v>82</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>80</v>
@@ -9308,27 +9311,27 @@
         <v>82</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AO60" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP60" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9354,16 +9357,16 @@
         <v>197</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="O61" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="P61" t="s" s="2">
         <v>82</v>
@@ -9388,13 +9391,13 @@
         <v>82</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>82</v>
@@ -9412,7 +9415,7 @@
         <v>82</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>80</v>
@@ -9421,7 +9424,7 @@
         <v>92</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>105</v>
@@ -9436,7 +9439,7 @@
         <v>106</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AO61" t="s" s="2">
         <v>82</v>
@@ -9447,14 +9450,14 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
@@ -9476,16 +9479,16 @@
         <v>197</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O62" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="P62" t="s" s="2">
         <v>82</v>
@@ -9510,13 +9513,13 @@
         <v>82</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>82</v>
@@ -9534,7 +9537,7 @@
         <v>82</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>80</v>
@@ -9552,27 +9555,27 @@
         <v>82</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AO62" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP62" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9598,16 +9601,16 @@
         <v>83</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="O63" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="P63" t="s" s="2">
         <v>82</v>
@@ -9656,7 +9659,7 @@
         <v>82</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>80</v>
@@ -9677,10 +9680,10 @@
         <v>82</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AO63" t="s" s="2">
         <v>82</v>

</xml_diff>